<commit_message>
Add sitemap for GSC
</commit_message>
<xml_diff>
--- a/catalogo.xlsx
+++ b/catalogo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/508ea63fb0320d71/Desktop/lojacocriativo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvia\OneDrive\Desktop\lojacocriativo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{78E1242E-9732-4814-86E7-6E260A1187DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CE04DB1-B2EF-498F-9125-BACA49C5CD36}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1570AC11-0448-4F97-B171-34909903FF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2595,8 +2595,8 @@
   </sheetPr>
   <dimension ref="A1:F304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
-      <selection activeCell="I230" sqref="I230"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C223" sqref="C223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>